<commit_message>
Implemented automatic persistence forecasting for wind
</commit_message>
<xml_diff>
--- a/data/RESERVE_settings.xlsx
+++ b/data/RESERVE_settings.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charles.gulian\PycharmProjects\RESERVE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F260AC-4E20-4FCE-8EC6-AB4EBABB7895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E60F992-154F-48C7-BEBC-4F153780ECC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RESERVE Settings" sheetId="1" r:id="rId1"/>
-    <sheet name="Input File Settings" sheetId="4" r:id="rId2"/>
+    <sheet name="Input Data Settings" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Value</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Forecast</t>
   </si>
   <si>
-    <t>Filename</t>
-  </si>
-  <si>
     <t>Load_forecast_5_min_ahead_processed.csv</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>Solar_forecast_15_min_ahead_processed.csv</t>
   </si>
   <si>
-    <t>Wind_forecast_15_min_ahead_processed.csv</t>
-  </si>
-  <si>
     <t>Feature</t>
   </si>
   <si>
@@ -133,7 +127,10 @@
     <t>Time difference in hours between time zone of power system and UTC</t>
   </si>
   <si>
-    <t>Use Persistence Forecast From Actual</t>
+    <t>persistence</t>
+  </si>
+  <si>
+    <t>Data Source</t>
   </si>
 </sst>
 </file>
@@ -993,7 +990,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1004,7 +1001,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1015,7 +1012,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1">
         <v>42736</v>
@@ -1027,7 +1024,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -1035,10 +1032,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -1046,10 +1043,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
       </c>
       <c r="C6">
         <v>-119.4179</v>
@@ -1057,10 +1054,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
         <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
       </c>
       <c r="C7">
         <v>-8</v>
@@ -1073,46 +1070,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1129,13 +1123,10 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1152,13 +1143,10 @@
       <c r="F3">
         <v>3</v>
       </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1175,13 +1163,10 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -1198,13 +1183,10 @@
       <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -1221,13 +1203,10 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1243,9 +1222,6 @@
       </c>
       <c r="F7">
         <v>3</v>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created persistence forecasting method for solar using theoretical clear sky output.
</commit_message>
<xml_diff>
--- a/data/RESERVE_settings.xlsx
+++ b/data/RESERVE_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charles.gulian\PycharmProjects\RESERVE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E60F992-154F-48C7-BEBC-4F153780ECC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5749C3C2-B12E-410E-897B-F66518E4817E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15336" yWindow="1044" windowWidth="14400" windowHeight="8328" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RESERVE Settings" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Value</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Load_forecast_15_min_ahead_processed.csv</t>
   </si>
   <si>
-    <t>Solar_forecast_15_min_ahead_processed.csv</t>
-  </si>
-  <si>
     <t>Feature</t>
   </si>
   <si>
@@ -131,6 +128,12 @@
   </si>
   <si>
     <t>Data Source</t>
+  </si>
+  <si>
+    <t>LATITUDE</t>
+  </si>
+  <si>
+    <t>Approximate latitude of power system</t>
   </si>
 </sst>
 </file>
@@ -972,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -990,7 +993,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1001,7 +1004,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1012,7 +1015,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1">
         <v>42736</v>
@@ -1024,7 +1027,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -1032,10 +1035,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -1043,28 +1046,40 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C6">
-        <v>-119.4179</v>
+        <v>36.677700000000002</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
       <c r="C7">
+        <v>-119.4179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
         <v>-8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1073,7 +1088,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1086,22 +1101,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1166,7 +1181,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -1206,7 +1221,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Minor changes to data_preprocessing_into_inputs.py
</commit_message>
<xml_diff>
--- a/data/RESERVE_settings.xlsx
+++ b/data/RESERVE_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charles.gulian\PycharmProjects\RESERVE\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5749C3C2-B12E-410E-897B-F66518E4817E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1060523A-C355-4A1D-8B69-C2A66A65BA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15336" yWindow="1044" windowWidth="14400" windowHeight="8328" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-1608" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RESERVE Settings" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,6 @@
     <t>ANCHOR_DATE</t>
   </si>
   <si>
-    <t>rescue_v1_4_manually_cleaned</t>
-  </si>
-  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -70,18 +67,6 @@
     <t>Forecast</t>
   </si>
   <si>
-    <t>Load_forecast_5_min_ahead_processed.csv</t>
-  </si>
-  <si>
-    <t>Wind_forecast_5_min_ahead_processed.csv</t>
-  </si>
-  <si>
-    <t>Solar_forecast_5_min_ahead_processed.csv</t>
-  </si>
-  <si>
-    <t>Load_forecast_15_min_ahead_processed.csv</t>
-  </si>
-  <si>
     <t>Feature</t>
   </si>
   <si>
@@ -134,6 +119,21 @@
   </si>
   <si>
     <t>Approximate latitude of power system</t>
+  </si>
+  <si>
+    <t>PSE_RTPD_load_forecast.csv</t>
+  </si>
+  <si>
+    <t>PSE_RTD_load_forecast.csv</t>
+  </si>
+  <si>
+    <t>PSE_wind_5_minute_actuals.csv</t>
+  </si>
+  <si>
+    <t>PSE_solar_5_minute_actuals.csv</t>
+  </si>
+  <si>
+    <t>reserve_PSE_2022</t>
   </si>
 </sst>
 </file>
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -990,10 +990,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1001,13 +1001,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1015,19 +1015,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1">
-        <v>42736</v>
+        <v>43466</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -1035,10 +1035,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -1046,32 +1046,32 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C6">
-        <v>36.677700000000002</v>
+        <v>47.543999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>-119.4179</v>
+        <v>-120.411</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>-8</v>
@@ -1087,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1101,33 +1101,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>-6</v>
@@ -1141,13 +1141,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>-6</v>
@@ -1161,13 +1161,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>-6</v>
@@ -1181,13 +1181,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>-6</v>
@@ -1201,13 +1201,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>-6</v>
@@ -1221,13 +1221,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <v>-6</v>

</xml_diff>